<commit_message>
fixing typos in rnaseq
</commit_message>
<xml_diff>
--- a/rnaSample/rnaSample_H.BROWN_10.23.20.xlsx
+++ b/rnaSample/rnaSample_H.BROWN_10.23.20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="13">
   <si>
     <t xml:space="preserve">harvestDate</t>
   </si>
@@ -56,16 +56,20 @@
   </si>
   <si>
     <t xml:space="preserve">TRIzol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -87,6 +91,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,8 +142,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -156,12 +171,15 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -190,7 +208,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
@@ -210,13 +228,13 @@
         <v>1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
@@ -236,13 +254,13 @@
         <v>2</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
@@ -262,13 +280,13 @@
         <v>3</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
@@ -288,13 +306,13 @@
         <v>4</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>8</v>
       </c>
@@ -314,13 +332,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>8</v>
       </c>
@@ -340,13 +358,13 @@
         <v>6</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>8</v>
       </c>
@@ -366,13 +384,13 @@
         <v>7</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>8</v>
       </c>
@@ -392,13 +410,13 @@
         <v>8</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>8</v>
       </c>
@@ -418,13 +436,13 @@
         <v>9</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>8</v>
       </c>
@@ -444,13 +462,13 @@
         <v>10</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>8</v>
       </c>
@@ -470,13 +488,13 @@
         <v>11</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>8</v>
       </c>
@@ -496,13 +514,13 @@
         <v>12</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>8</v>
       </c>
@@ -522,13 +540,13 @@
         <v>13</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>8</v>
       </c>
@@ -548,13 +566,13 @@
         <v>14</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>8</v>
       </c>
@@ -574,13 +592,13 @@
         <v>15</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>8</v>
       </c>
@@ -600,13 +618,13 @@
         <v>16</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>8</v>
       </c>
@@ -626,13 +644,13 @@
         <v>17</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>8</v>
       </c>
@@ -652,13 +670,13 @@
         <v>18</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>8</v>
       </c>
@@ -678,13 +696,13 @@
         <v>19</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>8</v>
       </c>
@@ -704,13 +722,13 @@
         <v>20</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>8</v>
       </c>
@@ -730,13 +748,13 @@
         <v>21</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>8</v>
       </c>
@@ -756,13 +774,13 @@
         <v>22</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>8</v>
       </c>
@@ -782,13 +800,13 @@
         <v>23</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>8</v>
       </c>
@@ -808,13 +826,13 @@
         <v>24</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>8</v>
       </c>
@@ -834,13 +852,13 @@
         <v>25</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>8</v>
       </c>
@@ -860,13 +878,13 @@
         <v>26</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>8</v>
       </c>
@@ -886,13 +904,13 @@
         <v>27</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>8</v>
       </c>
@@ -912,13 +930,13 @@
         <v>28</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>8</v>
       </c>
@@ -938,13 +956,13 @@
         <v>29</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>8</v>
       </c>
@@ -964,13 +982,13 @@
         <v>30</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>8</v>
       </c>
@@ -990,13 +1008,13 @@
         <v>31</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>8</v>
       </c>
@@ -1016,10 +1034,10 @@
         <v>32</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>